<commit_message>
Add new Title and Add "No Evaluation" to Fig
</commit_message>
<xml_diff>
--- a/data/literature.xlsx
+++ b/data/literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCode\DesignScienceResearch_LiteraturReview\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3215D41-B1CB-42E5-9285-A0BF120DA4B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95245E28-9E8A-4B59-A3FB-4F4CD2AA0BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="510">
   <si>
     <t>Artefakte</t>
   </si>
@@ -1565,6 +1565,9 @@
   <si>
     <t>Konferenz-ID</t>
   </si>
+  <si>
+    <t>Modell</t>
+  </si>
 </sst>
 </file>
 
@@ -2652,13 +2655,31 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2669,6 +2690,33 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2706,49 +2754,13 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2773,15 +2785,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3111,7 +3114,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BH20" sqref="BH20"/>
+      <selection pane="bottomLeft" activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3147,62 +3150,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:163" s="59" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="269"/>
-      <c r="B1" s="270"/>
-      <c r="C1" s="270"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="254" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
-      <c r="M1" s="255"/>
-      <c r="N1" s="255"/>
-      <c r="O1" s="255"/>
-      <c r="P1" s="255"/>
-      <c r="Q1" s="255"/>
-      <c r="R1" s="255"/>
-      <c r="S1" s="255"/>
-      <c r="T1" s="255"/>
-      <c r="U1" s="255"/>
-      <c r="V1" s="255"/>
-      <c r="W1" s="255"/>
-      <c r="X1" s="255"/>
-      <c r="Y1" s="255"/>
-      <c r="Z1" s="255"/>
-      <c r="AA1" s="255"/>
-      <c r="AB1" s="255"/>
-      <c r="AC1" s="255"/>
-      <c r="AD1" s="255"/>
-      <c r="AE1" s="256"/>
-      <c r="AF1" s="254" t="s">
+      <c r="A1" s="251"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="253"/>
+      <c r="E1" s="260" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="261"/>
+      <c r="L1" s="261"/>
+      <c r="M1" s="261"/>
+      <c r="N1" s="261"/>
+      <c r="O1" s="261"/>
+      <c r="P1" s="261"/>
+      <c r="Q1" s="261"/>
+      <c r="R1" s="261"/>
+      <c r="S1" s="261"/>
+      <c r="T1" s="261"/>
+      <c r="U1" s="261"/>
+      <c r="V1" s="261"/>
+      <c r="W1" s="261"/>
+      <c r="X1" s="261"/>
+      <c r="Y1" s="261"/>
+      <c r="Z1" s="261"/>
+      <c r="AA1" s="261"/>
+      <c r="AB1" s="261"/>
+      <c r="AC1" s="261"/>
+      <c r="AD1" s="261"/>
+      <c r="AE1" s="262"/>
+      <c r="AF1" s="260" t="s">
         <v>1</v>
       </c>
-      <c r="AG1" s="255"/>
-      <c r="AH1" s="255"/>
-      <c r="AI1" s="255"/>
-      <c r="AJ1" s="255"/>
-      <c r="AK1" s="255"/>
-      <c r="AL1" s="255"/>
-      <c r="AM1" s="255"/>
-      <c r="AN1" s="255"/>
-      <c r="AO1" s="255"/>
-      <c r="AP1" s="255"/>
-      <c r="AQ1" s="255"/>
-      <c r="AR1" s="255"/>
-      <c r="AS1" s="255"/>
-      <c r="AT1" s="255"/>
-      <c r="AU1" s="255"/>
-      <c r="AV1" s="255"/>
-      <c r="AW1" s="255"/>
-      <c r="AX1" s="255"/>
-      <c r="AY1" s="255"/>
-      <c r="AZ1" s="256"/>
+      <c r="AG1" s="261"/>
+      <c r="AH1" s="261"/>
+      <c r="AI1" s="261"/>
+      <c r="AJ1" s="261"/>
+      <c r="AK1" s="261"/>
+      <c r="AL1" s="261"/>
+      <c r="AM1" s="261"/>
+      <c r="AN1" s="261"/>
+      <c r="AO1" s="261"/>
+      <c r="AP1" s="261"/>
+      <c r="AQ1" s="261"/>
+      <c r="AR1" s="261"/>
+      <c r="AS1" s="261"/>
+      <c r="AT1" s="261"/>
+      <c r="AU1" s="261"/>
+      <c r="AV1" s="261"/>
+      <c r="AW1" s="261"/>
+      <c r="AX1" s="261"/>
+      <c r="AY1" s="261"/>
+      <c r="AZ1" s="262"/>
       <c r="BA1" s="180" t="s">
         <v>84</v>
       </c>
@@ -3332,72 +3335,72 @@
       <c r="D2" s="185" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="281" t="s">
+      <c r="E2" s="266" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="282"/>
-      <c r="G2" s="282"/>
-      <c r="H2" s="282"/>
-      <c r="I2" s="283"/>
-      <c r="J2" s="272" t="s">
+      <c r="F2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
+      <c r="J2" s="254" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="273"/>
-      <c r="L2" s="273"/>
-      <c r="M2" s="273"/>
-      <c r="N2" s="274"/>
-      <c r="O2" s="275" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="276"/>
-      <c r="Q2" s="276"/>
-      <c r="R2" s="276"/>
-      <c r="S2" s="276"/>
-      <c r="T2" s="276"/>
-      <c r="U2" s="276"/>
-      <c r="V2" s="276"/>
-      <c r="W2" s="276"/>
-      <c r="X2" s="276"/>
-      <c r="Y2" s="276"/>
-      <c r="Z2" s="277"/>
-      <c r="AA2" s="278" t="s">
+      <c r="K2" s="255"/>
+      <c r="L2" s="255"/>
+      <c r="M2" s="255"/>
+      <c r="N2" s="256"/>
+      <c r="O2" s="257" t="s">
+        <v>509</v>
+      </c>
+      <c r="P2" s="258"/>
+      <c r="Q2" s="258"/>
+      <c r="R2" s="258"/>
+      <c r="S2" s="258"/>
+      <c r="T2" s="258"/>
+      <c r="U2" s="258"/>
+      <c r="V2" s="258"/>
+      <c r="W2" s="258"/>
+      <c r="X2" s="258"/>
+      <c r="Y2" s="258"/>
+      <c r="Z2" s="259"/>
+      <c r="AA2" s="263" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="279"/>
-      <c r="AC2" s="279"/>
-      <c r="AD2" s="279"/>
-      <c r="AE2" s="280"/>
-      <c r="AF2" s="257" t="s">
+      <c r="AB2" s="264"/>
+      <c r="AC2" s="264"/>
+      <c r="AD2" s="264"/>
+      <c r="AE2" s="265"/>
+      <c r="AF2" s="272" t="s">
         <v>8</v>
       </c>
-      <c r="AG2" s="258"/>
-      <c r="AH2" s="258"/>
-      <c r="AI2" s="258"/>
-      <c r="AJ2" s="258"/>
-      <c r="AK2" s="259"/>
-      <c r="AL2" s="260" t="s">
+      <c r="AG2" s="273"/>
+      <c r="AH2" s="273"/>
+      <c r="AI2" s="273"/>
+      <c r="AJ2" s="273"/>
+      <c r="AK2" s="274"/>
+      <c r="AL2" s="275" t="s">
         <v>9</v>
       </c>
-      <c r="AM2" s="261"/>
-      <c r="AN2" s="261"/>
-      <c r="AO2" s="261"/>
-      <c r="AP2" s="262"/>
-      <c r="AQ2" s="263" t="s">
+      <c r="AM2" s="276"/>
+      <c r="AN2" s="276"/>
+      <c r="AO2" s="276"/>
+      <c r="AP2" s="277"/>
+      <c r="AQ2" s="278" t="s">
         <v>10</v>
       </c>
-      <c r="AR2" s="264"/>
-      <c r="AS2" s="264"/>
-      <c r="AT2" s="265"/>
-      <c r="AU2" s="266" t="s">
+      <c r="AR2" s="279"/>
+      <c r="AS2" s="279"/>
+      <c r="AT2" s="280"/>
+      <c r="AU2" s="281" t="s">
         <v>11</v>
       </c>
-      <c r="AV2" s="267"/>
-      <c r="AW2" s="268"/>
-      <c r="AX2" s="251" t="s">
+      <c r="AV2" s="282"/>
+      <c r="AW2" s="283"/>
+      <c r="AX2" s="269" t="s">
         <v>12</v>
       </c>
-      <c r="AY2" s="252"/>
-      <c r="AZ2" s="253"/>
+      <c r="AY2" s="270"/>
+      <c r="AZ2" s="271"/>
       <c r="BA2" s="186" t="s">
         <v>84</v>
       </c>
@@ -43409,18 +43412,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AX2:AZ2"/>
+    <mergeCell ref="AF1:AZ1"/>
+    <mergeCell ref="AF2:AK2"/>
+    <mergeCell ref="AL2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AU2:AW2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="J2:N2"/>
     <mergeCell ref="O2:Z2"/>
     <mergeCell ref="E1:AE1"/>
     <mergeCell ref="AA2:AE2"/>
     <mergeCell ref="E2:I2"/>
-    <mergeCell ref="AX2:AZ2"/>
-    <mergeCell ref="AF1:AZ1"/>
-    <mergeCell ref="AF2:AK2"/>
-    <mergeCell ref="AL2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AU2:AW2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -43488,60 +43491,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:160" s="59" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="269"/>
-      <c r="B1" s="271"/>
-      <c r="C1" s="285" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-      <c r="P1" s="285"/>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="285"/>
-      <c r="S1" s="285"/>
-      <c r="T1" s="285"/>
-      <c r="U1" s="285"/>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
-      <c r="X1" s="285"/>
-      <c r="Y1" s="285"/>
-      <c r="Z1" s="285"/>
-      <c r="AA1" s="285"/>
-      <c r="AB1" s="285"/>
-      <c r="AC1" s="285"/>
-      <c r="AD1" s="285" t="s">
+      <c r="A1" s="251"/>
+      <c r="B1" s="253"/>
+      <c r="C1" s="288" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="288"/>
+      <c r="P1" s="288"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="288"/>
+      <c r="S1" s="288"/>
+      <c r="T1" s="288"/>
+      <c r="U1" s="288"/>
+      <c r="V1" s="288"/>
+      <c r="W1" s="288"/>
+      <c r="X1" s="288"/>
+      <c r="Y1" s="288"/>
+      <c r="Z1" s="288"/>
+      <c r="AA1" s="288"/>
+      <c r="AB1" s="288"/>
+      <c r="AC1" s="288"/>
+      <c r="AD1" s="288" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="285"/>
-      <c r="AF1" s="285"/>
-      <c r="AG1" s="285"/>
-      <c r="AH1" s="285"/>
-      <c r="AI1" s="285"/>
-      <c r="AJ1" s="285"/>
-      <c r="AK1" s="285"/>
-      <c r="AL1" s="285"/>
-      <c r="AM1" s="285"/>
-      <c r="AN1" s="285"/>
-      <c r="AO1" s="285"/>
-      <c r="AP1" s="285"/>
-      <c r="AQ1" s="285"/>
-      <c r="AR1" s="285"/>
-      <c r="AS1" s="285"/>
-      <c r="AT1" s="285"/>
-      <c r="AU1" s="285"/>
-      <c r="AV1" s="285"/>
-      <c r="AW1" s="285"/>
-      <c r="AX1" s="285"/>
+      <c r="AE1" s="288"/>
+      <c r="AF1" s="288"/>
+      <c r="AG1" s="288"/>
+      <c r="AH1" s="288"/>
+      <c r="AI1" s="288"/>
+      <c r="AJ1" s="288"/>
+      <c r="AK1" s="288"/>
+      <c r="AL1" s="288"/>
+      <c r="AM1" s="288"/>
+      <c r="AN1" s="288"/>
+      <c r="AO1" s="288"/>
+      <c r="AP1" s="288"/>
+      <c r="AQ1" s="288"/>
+      <c r="AR1" s="288"/>
+      <c r="AS1" s="288"/>
+      <c r="AT1" s="288"/>
+      <c r="AU1" s="288"/>
+      <c r="AV1" s="288"/>
+      <c r="AW1" s="288"/>
+      <c r="AX1" s="288"/>
       <c r="AY1" s="11" t="s">
         <v>77</v>
       </c>
@@ -43662,72 +43665,72 @@
       <c r="B2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="293" t="s">
+      <c r="C2" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293"/>
-      <c r="H2" s="294" t="s">
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="286" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="M2" s="286" t="s">
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
+      <c r="K2" s="286"/>
+      <c r="L2" s="286"/>
+      <c r="M2" s="289" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="286"/>
-      <c r="R2" s="286"/>
-      <c r="S2" s="286"/>
-      <c r="T2" s="286"/>
-      <c r="U2" s="286"/>
-      <c r="V2" s="286"/>
-      <c r="W2" s="286"/>
-      <c r="X2" s="286"/>
-      <c r="Y2" s="287" t="s">
+      <c r="N2" s="289"/>
+      <c r="O2" s="289"/>
+      <c r="P2" s="289"/>
+      <c r="Q2" s="289"/>
+      <c r="R2" s="289"/>
+      <c r="S2" s="289"/>
+      <c r="T2" s="289"/>
+      <c r="U2" s="289"/>
+      <c r="V2" s="289"/>
+      <c r="W2" s="289"/>
+      <c r="X2" s="289"/>
+      <c r="Y2" s="290" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="287"/>
-      <c r="AA2" s="287"/>
-      <c r="AB2" s="287"/>
-      <c r="AC2" s="287"/>
-      <c r="AD2" s="288" t="s">
+      <c r="Z2" s="290"/>
+      <c r="AA2" s="290"/>
+      <c r="AB2" s="290"/>
+      <c r="AC2" s="290"/>
+      <c r="AD2" s="291" t="s">
         <v>8</v>
       </c>
-      <c r="AE2" s="288"/>
-      <c r="AF2" s="288"/>
-      <c r="AG2" s="288"/>
-      <c r="AH2" s="288"/>
-      <c r="AI2" s="288"/>
-      <c r="AJ2" s="289" t="s">
+      <c r="AE2" s="291"/>
+      <c r="AF2" s="291"/>
+      <c r="AG2" s="291"/>
+      <c r="AH2" s="291"/>
+      <c r="AI2" s="291"/>
+      <c r="AJ2" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" s="289"/>
-      <c r="AL2" s="289"/>
-      <c r="AM2" s="289"/>
-      <c r="AN2" s="289"/>
-      <c r="AO2" s="290" t="s">
+      <c r="AK2" s="292"/>
+      <c r="AL2" s="292"/>
+      <c r="AM2" s="292"/>
+      <c r="AN2" s="292"/>
+      <c r="AO2" s="293" t="s">
         <v>10</v>
       </c>
-      <c r="AP2" s="290"/>
-      <c r="AQ2" s="290"/>
-      <c r="AR2" s="290"/>
-      <c r="AS2" s="291" t="s">
+      <c r="AP2" s="293"/>
+      <c r="AQ2" s="293"/>
+      <c r="AR2" s="293"/>
+      <c r="AS2" s="294" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="291"/>
-      <c r="AU2" s="291"/>
-      <c r="AV2" s="284" t="s">
+      <c r="AT2" s="294"/>
+      <c r="AU2" s="294"/>
+      <c r="AV2" s="287" t="s">
         <v>12</v>
       </c>
-      <c r="AW2" s="284"/>
-      <c r="AX2" s="284"/>
+      <c r="AW2" s="287"/>
+      <c r="AX2" s="287"/>
       <c r="AY2" s="60" t="s">
         <v>77</v>
       </c>
@@ -44044,7 +44047,7 @@
       <c r="AY4" s="62"/>
     </row>
     <row r="5" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="292" t="s">
+      <c r="A5" s="284" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -44250,7 +44253,7 @@
       <c r="FD5" s="29"/>
     </row>
     <row r="6" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="292"/>
+      <c r="A6" s="284"/>
       <c r="B6" s="24" t="s">
         <v>56</v>
       </c>
@@ -44434,7 +44437,7 @@
       <c r="FD6" s="29"/>
     </row>
     <row r="7" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="292"/>
+      <c r="A7" s="284"/>
       <c r="B7" s="24" t="s">
         <v>65</v>
       </c>
@@ -44624,7 +44627,7 @@
       <c r="FD7" s="29"/>
     </row>
     <row r="8" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="292"/>
+      <c r="A8" s="284"/>
       <c r="B8" s="24" t="s">
         <v>63</v>
       </c>
@@ -44810,7 +44813,7 @@
       <c r="FD8" s="29"/>
     </row>
     <row r="9" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="292"/>
+      <c r="A9" s="284"/>
       <c r="B9" s="24" t="s">
         <v>62</v>
       </c>
@@ -44984,7 +44987,7 @@
       <c r="FD9" s="29"/>
     </row>
     <row r="10" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="292"/>
+      <c r="A10" s="284"/>
       <c r="B10" s="24" t="s">
         <v>69</v>
       </c>
@@ -45156,7 +45159,7 @@
       <c r="FD10" s="29"/>
     </row>
     <row r="11" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="292"/>
+      <c r="A11" s="284"/>
       <c r="B11" s="24" t="s">
         <v>58</v>
       </c>
@@ -45336,7 +45339,7 @@
       <c r="FD11" s="29"/>
     </row>
     <row r="12" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="292"/>
+      <c r="A12" s="284"/>
       <c r="B12" s="24" t="s">
         <v>57</v>
       </c>
@@ -45569,7 +45572,7 @@
       <c r="AY13" s="62"/>
     </row>
     <row r="14" spans="1:160" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="292" t="s">
+      <c r="A14" s="284" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -45649,7 +45652,7 @@
       <c r="AX14" s="49"/>
     </row>
     <row r="15" spans="1:160" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="292"/>
+      <c r="A15" s="284"/>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
@@ -45705,7 +45708,7 @@
       <c r="AX15" s="49"/>
     </row>
     <row r="16" spans="1:160" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="292"/>
+      <c r="A16" s="284"/>
       <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
@@ -45761,7 +45764,7 @@
       <c r="AX16" s="49"/>
     </row>
     <row r="17" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="292"/>
+      <c r="A17" s="284"/>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
@@ -45817,7 +45820,7 @@
       <c r="AX17" s="49"/>
     </row>
     <row r="18" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="292"/>
+      <c r="A18" s="284"/>
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
@@ -45873,7 +45876,7 @@
       <c r="AX18" s="49"/>
     </row>
     <row r="19" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="292"/>
+      <c r="A19" s="284"/>
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
@@ -45929,7 +45932,7 @@
       <c r="AX19" s="49"/>
     </row>
     <row r="20" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="292"/>
+      <c r="A20" s="284"/>
       <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
@@ -45985,7 +45988,7 @@
       <c r="AX20" s="49"/>
     </row>
     <row r="21" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="292"/>
+      <c r="A21" s="284"/>
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
@@ -46041,7 +46044,7 @@
       </c>
     </row>
     <row r="22" spans="1:51" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="292"/>
+      <c r="A22" s="284"/>
       <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
@@ -51624,11 +51627,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
     <mergeCell ref="AV2:AX2"/>
     <mergeCell ref="C1:AC1"/>
     <mergeCell ref="AD1:AX1"/>
@@ -51638,6 +51636,11 @@
     <mergeCell ref="AJ2:AN2"/>
     <mergeCell ref="AO2:AR2"/>
     <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions headings="1"/>
@@ -51695,58 +51698,58 @@
     <row r="1" spans="1:160" s="122" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="296"/>
       <c r="B1" s="297"/>
-      <c r="C1" s="285" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-      <c r="P1" s="285"/>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="285"/>
-      <c r="S1" s="285"/>
-      <c r="T1" s="285"/>
-      <c r="U1" s="285"/>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
-      <c r="X1" s="285"/>
-      <c r="Y1" s="285"/>
-      <c r="Z1" s="285"/>
-      <c r="AA1" s="285"/>
-      <c r="AB1" s="285"/>
-      <c r="AC1" s="285"/>
-      <c r="AD1" s="285" t="s">
+      <c r="C1" s="288" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="288"/>
+      <c r="P1" s="288"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="288"/>
+      <c r="S1" s="288"/>
+      <c r="T1" s="288"/>
+      <c r="U1" s="288"/>
+      <c r="V1" s="288"/>
+      <c r="W1" s="288"/>
+      <c r="X1" s="288"/>
+      <c r="Y1" s="288"/>
+      <c r="Z1" s="288"/>
+      <c r="AA1" s="288"/>
+      <c r="AB1" s="288"/>
+      <c r="AC1" s="288"/>
+      <c r="AD1" s="288" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="285"/>
-      <c r="AF1" s="285"/>
-      <c r="AG1" s="285"/>
-      <c r="AH1" s="285"/>
-      <c r="AI1" s="285"/>
-      <c r="AJ1" s="285"/>
-      <c r="AK1" s="285"/>
-      <c r="AL1" s="285"/>
-      <c r="AM1" s="285"/>
-      <c r="AN1" s="285"/>
-      <c r="AO1" s="285"/>
-      <c r="AP1" s="285"/>
-      <c r="AQ1" s="285"/>
-      <c r="AR1" s="285"/>
-      <c r="AS1" s="285"/>
-      <c r="AT1" s="285"/>
-      <c r="AU1" s="285"/>
-      <c r="AV1" s="285"/>
-      <c r="AW1" s="285"/>
-      <c r="AX1" s="285"/>
+      <c r="AE1" s="288"/>
+      <c r="AF1" s="288"/>
+      <c r="AG1" s="288"/>
+      <c r="AH1" s="288"/>
+      <c r="AI1" s="288"/>
+      <c r="AJ1" s="288"/>
+      <c r="AK1" s="288"/>
+      <c r="AL1" s="288"/>
+      <c r="AM1" s="288"/>
+      <c r="AN1" s="288"/>
+      <c r="AO1" s="288"/>
+      <c r="AP1" s="288"/>
+      <c r="AQ1" s="288"/>
+      <c r="AR1" s="288"/>
+      <c r="AS1" s="288"/>
+      <c r="AT1" s="288"/>
+      <c r="AU1" s="288"/>
+      <c r="AV1" s="288"/>
+      <c r="AW1" s="288"/>
+      <c r="AX1" s="288"/>
       <c r="AY1" s="118" t="s">
         <v>77</v>
       </c>
@@ -51867,72 +51870,72 @@
       <c r="B2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="293" t="s">
+      <c r="C2" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293"/>
-      <c r="H2" s="294" t="s">
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="286" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="M2" s="286" t="s">
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
+      <c r="K2" s="286"/>
+      <c r="L2" s="286"/>
+      <c r="M2" s="289" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="286"/>
-      <c r="R2" s="286"/>
-      <c r="S2" s="286"/>
-      <c r="T2" s="286"/>
-      <c r="U2" s="286"/>
-      <c r="V2" s="286"/>
-      <c r="W2" s="286"/>
-      <c r="X2" s="286"/>
-      <c r="Y2" s="287" t="s">
+      <c r="N2" s="289"/>
+      <c r="O2" s="289"/>
+      <c r="P2" s="289"/>
+      <c r="Q2" s="289"/>
+      <c r="R2" s="289"/>
+      <c r="S2" s="289"/>
+      <c r="T2" s="289"/>
+      <c r="U2" s="289"/>
+      <c r="V2" s="289"/>
+      <c r="W2" s="289"/>
+      <c r="X2" s="289"/>
+      <c r="Y2" s="290" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="287"/>
-      <c r="AA2" s="287"/>
-      <c r="AB2" s="287"/>
-      <c r="AC2" s="287"/>
-      <c r="AD2" s="288" t="s">
+      <c r="Z2" s="290"/>
+      <c r="AA2" s="290"/>
+      <c r="AB2" s="290"/>
+      <c r="AC2" s="290"/>
+      <c r="AD2" s="291" t="s">
         <v>8</v>
       </c>
-      <c r="AE2" s="288"/>
-      <c r="AF2" s="288"/>
-      <c r="AG2" s="288"/>
-      <c r="AH2" s="288"/>
-      <c r="AI2" s="288"/>
-      <c r="AJ2" s="289" t="s">
+      <c r="AE2" s="291"/>
+      <c r="AF2" s="291"/>
+      <c r="AG2" s="291"/>
+      <c r="AH2" s="291"/>
+      <c r="AI2" s="291"/>
+      <c r="AJ2" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" s="289"/>
-      <c r="AL2" s="289"/>
-      <c r="AM2" s="289"/>
-      <c r="AN2" s="289"/>
-      <c r="AO2" s="290" t="s">
+      <c r="AK2" s="292"/>
+      <c r="AL2" s="292"/>
+      <c r="AM2" s="292"/>
+      <c r="AN2" s="292"/>
+      <c r="AO2" s="293" t="s">
         <v>10</v>
       </c>
-      <c r="AP2" s="290"/>
-      <c r="AQ2" s="290"/>
-      <c r="AR2" s="290"/>
-      <c r="AS2" s="291" t="s">
+      <c r="AP2" s="293"/>
+      <c r="AQ2" s="293"/>
+      <c r="AR2" s="293"/>
+      <c r="AS2" s="294" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="291"/>
-      <c r="AU2" s="291"/>
-      <c r="AV2" s="284" t="s">
+      <c r="AT2" s="294"/>
+      <c r="AU2" s="294"/>
+      <c r="AV2" s="287" t="s">
         <v>12</v>
       </c>
-      <c r="AW2" s="284"/>
-      <c r="AX2" s="284"/>
+      <c r="AW2" s="287"/>
+      <c r="AX2" s="287"/>
       <c r="AY2" s="60" t="s">
         <v>77</v>
       </c>
@@ -61952,11 +61955,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
     <mergeCell ref="AV2:AX2"/>
     <mergeCell ref="C1:AC1"/>
     <mergeCell ref="AD1:AX1"/>
@@ -61966,6 +61964,11 @@
     <mergeCell ref="AJ2:AN2"/>
     <mergeCell ref="AO2:AR2"/>
     <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -62013,60 +62016,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:160" s="59" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="269"/>
-      <c r="B1" s="271"/>
-      <c r="C1" s="285" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-      <c r="P1" s="285"/>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="285"/>
-      <c r="S1" s="285"/>
-      <c r="T1" s="285"/>
-      <c r="U1" s="285"/>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
-      <c r="X1" s="285"/>
-      <c r="Y1" s="285"/>
-      <c r="Z1" s="285"/>
-      <c r="AA1" s="285"/>
-      <c r="AB1" s="285"/>
-      <c r="AC1" s="285"/>
-      <c r="AD1" s="285" t="s">
+      <c r="A1" s="251"/>
+      <c r="B1" s="253"/>
+      <c r="C1" s="288" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="288"/>
+      <c r="P1" s="288"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="288"/>
+      <c r="S1" s="288"/>
+      <c r="T1" s="288"/>
+      <c r="U1" s="288"/>
+      <c r="V1" s="288"/>
+      <c r="W1" s="288"/>
+      <c r="X1" s="288"/>
+      <c r="Y1" s="288"/>
+      <c r="Z1" s="288"/>
+      <c r="AA1" s="288"/>
+      <c r="AB1" s="288"/>
+      <c r="AC1" s="288"/>
+      <c r="AD1" s="288" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="285"/>
-      <c r="AF1" s="285"/>
-      <c r="AG1" s="285"/>
-      <c r="AH1" s="285"/>
-      <c r="AI1" s="285"/>
-      <c r="AJ1" s="285"/>
-      <c r="AK1" s="285"/>
-      <c r="AL1" s="285"/>
-      <c r="AM1" s="285"/>
-      <c r="AN1" s="285"/>
-      <c r="AO1" s="285"/>
-      <c r="AP1" s="285"/>
-      <c r="AQ1" s="285"/>
-      <c r="AR1" s="285"/>
-      <c r="AS1" s="285"/>
-      <c r="AT1" s="285"/>
-      <c r="AU1" s="285"/>
-      <c r="AV1" s="285"/>
-      <c r="AW1" s="285"/>
-      <c r="AX1" s="285"/>
+      <c r="AE1" s="288"/>
+      <c r="AF1" s="288"/>
+      <c r="AG1" s="288"/>
+      <c r="AH1" s="288"/>
+      <c r="AI1" s="288"/>
+      <c r="AJ1" s="288"/>
+      <c r="AK1" s="288"/>
+      <c r="AL1" s="288"/>
+      <c r="AM1" s="288"/>
+      <c r="AN1" s="288"/>
+      <c r="AO1" s="288"/>
+      <c r="AP1" s="288"/>
+      <c r="AQ1" s="288"/>
+      <c r="AR1" s="288"/>
+      <c r="AS1" s="288"/>
+      <c r="AT1" s="288"/>
+      <c r="AU1" s="288"/>
+      <c r="AV1" s="288"/>
+      <c r="AW1" s="288"/>
+      <c r="AX1" s="288"/>
       <c r="AY1" s="11" t="s">
         <v>77</v>
       </c>
@@ -62187,72 +62190,72 @@
       <c r="B2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="293" t="s">
+      <c r="C2" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293"/>
-      <c r="H2" s="294" t="s">
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="286" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="M2" s="286" t="s">
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
+      <c r="K2" s="286"/>
+      <c r="L2" s="286"/>
+      <c r="M2" s="289" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="286"/>
-      <c r="R2" s="286"/>
-      <c r="S2" s="286"/>
-      <c r="T2" s="286"/>
-      <c r="U2" s="286"/>
-      <c r="V2" s="286"/>
-      <c r="W2" s="286"/>
-      <c r="X2" s="286"/>
-      <c r="Y2" s="287" t="s">
+      <c r="N2" s="289"/>
+      <c r="O2" s="289"/>
+      <c r="P2" s="289"/>
+      <c r="Q2" s="289"/>
+      <c r="R2" s="289"/>
+      <c r="S2" s="289"/>
+      <c r="T2" s="289"/>
+      <c r="U2" s="289"/>
+      <c r="V2" s="289"/>
+      <c r="W2" s="289"/>
+      <c r="X2" s="289"/>
+      <c r="Y2" s="290" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="287"/>
-      <c r="AA2" s="287"/>
-      <c r="AB2" s="287"/>
-      <c r="AC2" s="287"/>
-      <c r="AD2" s="288" t="s">
+      <c r="Z2" s="290"/>
+      <c r="AA2" s="290"/>
+      <c r="AB2" s="290"/>
+      <c r="AC2" s="290"/>
+      <c r="AD2" s="291" t="s">
         <v>8</v>
       </c>
-      <c r="AE2" s="288"/>
-      <c r="AF2" s="288"/>
-      <c r="AG2" s="288"/>
-      <c r="AH2" s="288"/>
-      <c r="AI2" s="288"/>
-      <c r="AJ2" s="289" t="s">
+      <c r="AE2" s="291"/>
+      <c r="AF2" s="291"/>
+      <c r="AG2" s="291"/>
+      <c r="AH2" s="291"/>
+      <c r="AI2" s="291"/>
+      <c r="AJ2" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" s="289"/>
-      <c r="AL2" s="289"/>
-      <c r="AM2" s="289"/>
-      <c r="AN2" s="289"/>
-      <c r="AO2" s="290" t="s">
+      <c r="AK2" s="292"/>
+      <c r="AL2" s="292"/>
+      <c r="AM2" s="292"/>
+      <c r="AN2" s="292"/>
+      <c r="AO2" s="293" t="s">
         <v>10</v>
       </c>
-      <c r="AP2" s="290"/>
-      <c r="AQ2" s="290"/>
-      <c r="AR2" s="290"/>
-      <c r="AS2" s="291" t="s">
+      <c r="AP2" s="293"/>
+      <c r="AQ2" s="293"/>
+      <c r="AR2" s="293"/>
+      <c r="AS2" s="294" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="291"/>
-      <c r="AU2" s="291"/>
-      <c r="AV2" s="284" t="s">
+      <c r="AT2" s="294"/>
+      <c r="AU2" s="294"/>
+      <c r="AV2" s="287" t="s">
         <v>12</v>
       </c>
-      <c r="AW2" s="284"/>
-      <c r="AX2" s="284"/>
+      <c r="AW2" s="287"/>
+      <c r="AX2" s="287"/>
       <c r="AY2" s="60" t="s">
         <v>77</v>
       </c>
@@ -62569,7 +62572,7 @@
       <c r="AY4" s="62"/>
     </row>
     <row r="5" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="292" t="s">
+      <c r="A5" s="284" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -62775,7 +62778,7 @@
       <c r="FD5" s="29"/>
     </row>
     <row r="6" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="292"/>
+      <c r="A6" s="284"/>
       <c r="B6" s="24" t="s">
         <v>56</v>
       </c>
@@ -62959,7 +62962,7 @@
       <c r="FD6" s="29"/>
     </row>
     <row r="7" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="292"/>
+      <c r="A7" s="284"/>
       <c r="B7" s="24" t="s">
         <v>65</v>
       </c>
@@ -63149,7 +63152,7 @@
       <c r="FD7" s="29"/>
     </row>
     <row r="8" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="292"/>
+      <c r="A8" s="284"/>
       <c r="B8" s="24" t="s">
         <v>63</v>
       </c>
@@ -63335,7 +63338,7 @@
       <c r="FD8" s="29"/>
     </row>
     <row r="9" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="292"/>
+      <c r="A9" s="284"/>
       <c r="B9" s="24" t="s">
         <v>62</v>
       </c>
@@ -63509,7 +63512,7 @@
       <c r="FD9" s="29"/>
     </row>
     <row r="10" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="292"/>
+      <c r="A10" s="284"/>
       <c r="B10" s="24" t="s">
         <v>69</v>
       </c>
@@ -63681,7 +63684,7 @@
       <c r="FD10" s="29"/>
     </row>
     <row r="11" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="292"/>
+      <c r="A11" s="284"/>
       <c r="B11" s="24" t="s">
         <v>58</v>
       </c>
@@ -63861,7 +63864,7 @@
       <c r="FD11" s="29"/>
     </row>
     <row r="12" spans="1:160" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="292"/>
+      <c r="A12" s="284"/>
       <c r="B12" s="24" t="s">
         <v>57</v>
       </c>
@@ -64094,7 +64097,7 @@
       <c r="AY13" s="62"/>
     </row>
     <row r="14" spans="1:160" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="292" t="s">
+      <c r="A14" s="284" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -64174,7 +64177,7 @@
       <c r="AX14" s="49"/>
     </row>
     <row r="15" spans="1:160" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="292"/>
+      <c r="A15" s="284"/>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
@@ -64230,7 +64233,7 @@
       <c r="AX15" s="49"/>
     </row>
     <row r="16" spans="1:160" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="292"/>
+      <c r="A16" s="284"/>
       <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
@@ -64286,7 +64289,7 @@
       <c r="AX16" s="49"/>
     </row>
     <row r="17" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="292"/>
+      <c r="A17" s="284"/>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
@@ -64342,7 +64345,7 @@
       <c r="AX17" s="49"/>
     </row>
     <row r="18" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="292"/>
+      <c r="A18" s="284"/>
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
@@ -64398,7 +64401,7 @@
       <c r="AX18" s="49"/>
     </row>
     <row r="19" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="292"/>
+      <c r="A19" s="284"/>
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
@@ -64454,7 +64457,7 @@
       <c r="AX19" s="49"/>
     </row>
     <row r="20" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="292"/>
+      <c r="A20" s="284"/>
       <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
@@ -64510,7 +64513,7 @@
       <c r="AX20" s="49"/>
     </row>
     <row r="21" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="292"/>
+      <c r="A21" s="284"/>
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
@@ -64566,7 +64569,7 @@
       </c>
     </row>
     <row r="22" spans="1:51" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="292"/>
+      <c r="A22" s="284"/>
       <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
@@ -70689,11 +70692,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
     <mergeCell ref="AV2:AX2"/>
     <mergeCell ref="C1:AC1"/>
     <mergeCell ref="AD1:AX1"/>
@@ -70703,6 +70701,11 @@
     <mergeCell ref="AJ2:AN2"/>
     <mergeCell ref="AO2:AR2"/>
     <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -70711,6 +70714,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E2C36908031EAA4DBA4B215FF24AC16B" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="25d4e3628e74548e003023a6e3d05b60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="626cd67d-102d-46d0-ac37-3e6bebf97187" xmlns:ns4="462a4cbc-85ef-4c28-ad24-c497397070e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d17c4b31f0b9c9b8b8eca0bdaf2f3e1" ns3:_="" ns4:_="">
     <xsd:import namespace="626cd67d-102d-46d0-ac37-3e6bebf97187"/>
@@ -70881,36 +70899,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2531E1F-36F0-4D6F-8959-A821D9D1B4F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F08EF8D-CDD2-499D-902D-DE25C019B585}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="626cd67d-102d-46d0-ac37-3e6bebf97187"/>
-    <ds:schemaRef ds:uri="462a4cbc-85ef-4c28-ad24-c497397070e6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -70933,9 +70925,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F08EF8D-CDD2-499D-902D-DE25C019B585}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2531E1F-36F0-4D6F-8959-A821D9D1B4F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="626cd67d-102d-46d0-ac37-3e6bebf97187"/>
+    <ds:schemaRef ds:uri="462a4cbc-85ef-4c28-ad24-c497397070e6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>